<commit_message>
Regression test for all software versions. upon begining test update the SW Version and FRS version
</commit_message>
<xml_diff>
--- a/winter/Neo-Koolaire Regression Test.xlsx
+++ b/winter/Neo-Koolaire Regression Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>Pass</t>
   </si>
@@ -53,15 +53,9 @@
     <t>Validation Execution Summary</t>
   </si>
   <si>
-    <t>Testing 2.62 Reference: FRS D-11010_03 Neo-Koolaire 2018_FRS</t>
-  </si>
-  <si>
     <t>Section</t>
   </si>
   <si>
-    <t>Step</t>
-  </si>
-  <si>
     <t>TP pg.</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
   </si>
   <si>
     <t>Req Update</t>
-  </si>
-  <si>
-    <t>14.1, 14.2</t>
   </si>
   <si>
     <t>Initial Start-up (Ice Machine State 1)</t>
@@ -482,9 +473,6 @@
     <t>Validate that pressing the ON/OFF button on the UI when in delay mode will cancel the delay mode, turn off delay LEDs and start an initial start-up cycle.</t>
   </si>
   <si>
-    <t>14.11.1</t>
-  </si>
-  <si>
     <t>Safety Limit 1: Long Freeze Cycle</t>
   </si>
   <si>
@@ -503,9 +491,6 @@
     <t>Verify that the safety limit 1 LED on the board shall flash once on restart and shall continue to do so until 100 freeze cycles less than 45 minutes  have been counted.</t>
   </si>
   <si>
-    <t>14.11.2</t>
-  </si>
-  <si>
     <t>Safety Limit 2: Long Harvest Cycle</t>
   </si>
   <si>
@@ -527,9 +512,6 @@
     <t>Verify that the safety limit 2 LED on the board shall flash twice on restart and shall continue to do so until 100 harvest cycles less than 7 minutes have been counted.</t>
   </si>
   <si>
-    <t>14.11.3</t>
-  </si>
-  <si>
     <t>Safety Limit 3: Water Loss</t>
   </si>
   <si>
@@ -597,6 +579,45 @@
   </si>
   <si>
     <t>Validate that all inputs from the NEO UI are disabled during the test mode.</t>
+  </si>
+  <si>
+    <t>Test #</t>
+  </si>
+  <si>
+    <t>6.2.2</t>
+  </si>
+  <si>
+    <t>6.2.3</t>
+  </si>
+  <si>
+    <t>6.2.4</t>
+  </si>
+  <si>
+    <t>6.2.5</t>
+  </si>
+  <si>
+    <t>6.2.6</t>
+  </si>
+  <si>
+    <t>6.2.7</t>
+  </si>
+  <si>
+    <t>6.2.8</t>
+  </si>
+  <si>
+    <t>6.3.1</t>
+  </si>
+  <si>
+    <t>6.5.1</t>
+  </si>
+  <si>
+    <t>6.5.2</t>
+  </si>
+  <si>
+    <t>6.5.3</t>
+  </si>
+  <si>
+    <t>Testing ___ Reference: FRS D-11010_??</t>
   </si>
 </sst>
 </file>
@@ -796,7 +817,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -898,10 +919,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -922,10 +939,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -956,10 +969,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -999,7 +1008,247 @@
     <cellStyle name="Normal 2 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1872,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,7 +2205,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -1969,41 +2218,41 @@
     </row>
     <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="D7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="F7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="G7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="H7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="I7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="21"/>
@@ -2014,110 +2263,110 @@
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="28">
-        <v>2.62</v>
+        <v>3.11</v>
       </c>
       <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
       <c r="B10" s="24">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="28">
-        <v>2.62</v>
+        <v>3.11</v>
       </c>
       <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="24">
-        <v>1.3</v>
+        <v>3</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="28">
-        <v>2.62</v>
+        <v>3.11</v>
       </c>
       <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="24">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="28">
-        <v>2.62</v>
+        <v>3.11</v>
       </c>
       <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="24">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="28">
-        <v>2.62</v>
+        <v>3.11</v>
       </c>
       <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>14.3</v>
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>155</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
       <c r="D15" s="19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E15" s="22"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
@@ -2125,93 +2374,93 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="24">
-        <v>2.1</v>
-      </c>
-      <c r="C16" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="C16" s="29"/>
       <c r="D16" s="26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="27"/>
-      <c r="F16" s="37">
-        <v>2.62</v>
+      <c r="F16" s="28">
+        <v>3.11</v>
       </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="24">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C17" s="30"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="29"/>
       <c r="D17" s="26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E17" s="27"/>
-      <c r="F17" s="37">
-        <v>2.62</v>
+      <c r="F17" s="28">
+        <v>3.11</v>
       </c>
       <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="24">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C18" s="30"/>
+        <v>3</v>
+      </c>
+      <c r="C18" s="29"/>
       <c r="D18" s="26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="37">
-        <v>2.62</v>
+      <c r="F18" s="28">
+        <v>3.11</v>
       </c>
       <c r="G18" s="29"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="24">
-        <v>2.4</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="38" t="s">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="36" t="s">
+        <v>27</v>
       </c>
       <c r="E19" s="27"/>
-      <c r="F19" s="37">
-        <v>2.62</v>
+      <c r="F19" s="28">
+        <v>3.11</v>
       </c>
       <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
-        <v>14.4</v>
+      <c r="A20" s="37"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="21"/>
       <c r="D21" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E21" s="22"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
@@ -2219,501 +2468,501 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="23">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C22" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="C22" s="29"/>
       <c r="D22" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E22" s="27"/>
-      <c r="F22" s="30">
-        <v>2.62</v>
+      <c r="F22" s="28">
+        <v>3.11</v>
       </c>
       <c r="G22" s="29"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="23">
-        <v>4.2</v>
-      </c>
-      <c r="C23" s="30"/>
+        <v>2</v>
+      </c>
+      <c r="C23" s="29"/>
       <c r="D23" s="26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E23" s="27"/>
-      <c r="F23" s="30">
-        <v>2.62</v>
+      <c r="F23" s="28">
+        <v>3.11</v>
       </c>
       <c r="G23" s="29"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="23">
-        <v>4.3</v>
-      </c>
-      <c r="C24" s="30"/>
+        <v>3</v>
+      </c>
+      <c r="C24" s="29"/>
       <c r="D24" s="26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E24" s="27"/>
-      <c r="F24" s="30">
-        <v>2.62</v>
+      <c r="F24" s="28">
+        <v>3.11</v>
       </c>
       <c r="G24" s="29"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="23">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="38" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="36" t="s">
+        <v>32</v>
       </c>
       <c r="E25" s="27"/>
-      <c r="F25" s="30">
-        <v>2.62</v>
+      <c r="F25" s="28">
+        <v>3.11</v>
       </c>
       <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="23">
-        <v>4.5</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="38" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="36" t="s">
+        <v>33</v>
       </c>
       <c r="E26" s="27"/>
-      <c r="F26" s="30">
-        <v>2.62</v>
+      <c r="F26" s="28">
+        <v>3.11</v>
       </c>
       <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="23">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C27" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="C27" s="29"/>
       <c r="D27" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E27" s="27"/>
-      <c r="F27" s="30">
-        <v>2.62</v>
+      <c r="F27" s="28">
+        <v>3.11</v>
       </c>
       <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="23">
-        <v>4.7</v>
-      </c>
-      <c r="C28" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="C28" s="29"/>
       <c r="D28" s="26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E28" s="27"/>
-      <c r="F28" s="30">
-        <v>2.62</v>
+      <c r="F28" s="28">
+        <v>3.11</v>
       </c>
       <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="23">
-        <v>4.8</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="40" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="38" t="s">
+        <v>36</v>
       </c>
       <c r="E29" s="27"/>
-      <c r="F29" s="30">
-        <v>2.62</v>
+      <c r="F29" s="28">
+        <v>3.11</v>
       </c>
       <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="23">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="40" t="s">
-        <v>40</v>
+        <v>9</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="38" t="s">
+        <v>37</v>
       </c>
       <c r="E30" s="27"/>
-      <c r="F30" s="30">
-        <v>2.62</v>
+      <c r="F30" s="28">
+        <v>3.11</v>
       </c>
       <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
     </row>
     <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
-      <c r="B31" s="41">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="42" t="s">
-        <v>41</v>
+      <c r="B31" s="23">
+        <v>10</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="40" t="s">
+        <v>38</v>
       </c>
       <c r="E31" s="27"/>
-      <c r="F31" s="30">
-        <v>2.62</v>
+      <c r="F31" s="28">
+        <v>3.11</v>
       </c>
       <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="23">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="42" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="40" t="s">
+        <v>39</v>
       </c>
       <c r="E32" s="27"/>
-      <c r="F32" s="30">
-        <v>2.62</v>
+      <c r="F32" s="28">
+        <v>3.11</v>
       </c>
       <c r="G32" s="29"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
     </row>
     <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
-      <c r="B33" s="41">
-        <v>4.12</v>
-      </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="42" t="s">
-        <v>43</v>
+      <c r="B33" s="23">
+        <v>12</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="40" t="s">
+        <v>40</v>
       </c>
       <c r="E33" s="27"/>
-      <c r="F33" s="30">
-        <v>2.62</v>
+      <c r="F33" s="28">
+        <v>3.11</v>
       </c>
       <c r="G33" s="29"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="23">
-        <v>4.13</v>
-      </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="42" t="s">
-        <v>44</v>
+        <v>13</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="40" t="s">
+        <v>41</v>
       </c>
       <c r="E34" s="27"/>
-      <c r="F34" s="30">
-        <v>2.62</v>
+      <c r="F34" s="28">
+        <v>3.11</v>
       </c>
       <c r="G34" s="29"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
     </row>
     <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="23">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="42" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="E35" s="27"/>
-      <c r="F35" s="30">
-        <v>2.62</v>
+      <c r="F35" s="28">
+        <v>3.11</v>
       </c>
       <c r="G35" s="29"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
     </row>
     <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
-      <c r="B36" s="41">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="42" t="s">
-        <v>46</v>
+      <c r="B36" s="23">
+        <v>15</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="E36" s="27"/>
-      <c r="F36" s="30">
-        <v>2.62</v>
+      <c r="F36" s="28">
+        <v>3.11</v>
       </c>
       <c r="G36" s="29"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="23">
-        <v>4.16</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="30">
-        <v>2.62</v>
+        <v>16</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="41"/>
+      <c r="F37" s="28">
+        <v>3.11</v>
       </c>
       <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
-      <c r="B38" s="41">
-        <v>4.17</v>
-      </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="42" t="s">
-        <v>48</v>
+      <c r="B38" s="23">
+        <v>17</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="40" t="s">
+        <v>45</v>
       </c>
       <c r="E38" s="27"/>
-      <c r="F38" s="30">
-        <v>2.62</v>
+      <c r="F38" s="28">
+        <v>3.11</v>
       </c>
       <c r="G38" s="29"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
     </row>
     <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
       <c r="B39" s="23">
-        <v>4.1800000000000104</v>
-      </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="42" t="s">
-        <v>49</v>
+        <v>18</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="40" t="s">
+        <v>46</v>
       </c>
       <c r="E39" s="27"/>
-      <c r="F39" s="30">
-        <v>2.62</v>
+      <c r="F39" s="28">
+        <v>3.11</v>
       </c>
       <c r="G39" s="29"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
     </row>
     <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
-      <c r="B40" s="41">
-        <v>4.1900000000000102</v>
-      </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="42" t="s">
-        <v>50</v>
+      <c r="B40" s="23">
+        <v>19</v>
+      </c>
+      <c r="C40" s="29"/>
+      <c r="D40" s="40" t="s">
+        <v>47</v>
       </c>
       <c r="E40" s="27"/>
-      <c r="F40" s="30">
-        <v>2.62</v>
+      <c r="F40" s="28">
+        <v>3.11</v>
       </c>
       <c r="G40" s="29"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-    </row>
-    <row r="41" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
-      <c r="B41" s="41">
-        <v>4.2000000000000099</v>
-      </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="42" t="s">
-        <v>51</v>
+      <c r="B41" s="23">
+        <v>20</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="40" t="s">
+        <v>48</v>
       </c>
       <c r="E41" s="27"/>
-      <c r="F41" s="30">
-        <v>2.62</v>
+      <c r="F41" s="28">
+        <v>3.11</v>
       </c>
       <c r="G41" s="29"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="23"/>
       <c r="B42" s="23">
-        <v>4.2100000000000097</v>
-      </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="42" t="s">
-        <v>52</v>
+        <v>21</v>
+      </c>
+      <c r="C42" s="29"/>
+      <c r="D42" s="40" t="s">
+        <v>49</v>
       </c>
       <c r="E42" s="27"/>
-      <c r="F42" s="30">
-        <v>2.62</v>
+      <c r="F42" s="28">
+        <v>3.11</v>
       </c>
       <c r="G42" s="29"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
     </row>
     <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
-      <c r="B43" s="41">
-        <v>4.2200000000000104</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="38" t="s">
-        <v>53</v>
+      <c r="B43" s="23">
+        <v>22</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="36" t="s">
+        <v>50</v>
       </c>
       <c r="E43" s="27"/>
-      <c r="F43" s="30">
-        <v>2.62</v>
+      <c r="F43" s="28">
+        <v>3.11</v>
       </c>
       <c r="G43" s="29"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
     </row>
     <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="B44" s="23">
-        <v>4.2300000000000102</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="38" t="s">
-        <v>54</v>
+        <v>23</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="36" t="s">
+        <v>51</v>
       </c>
       <c r="E44" s="27"/>
-      <c r="F44" s="30">
-        <v>2.62</v>
+      <c r="F44" s="28">
+        <v>3.11</v>
       </c>
       <c r="G44" s="29"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
     </row>
     <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
-      <c r="B45" s="41">
-        <v>4.24000000000001</v>
-      </c>
-      <c r="C45" s="30"/>
-      <c r="D45" s="38" t="s">
-        <v>55</v>
+      <c r="B45" s="23">
+        <v>24</v>
+      </c>
+      <c r="C45" s="29"/>
+      <c r="D45" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="E45" s="27"/>
-      <c r="F45" s="30">
-        <v>2.62</v>
+      <c r="F45" s="28">
+        <v>3.11</v>
       </c>
       <c r="G45" s="29"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="23">
-        <v>4.2500000000000098</v>
-      </c>
-      <c r="C46" s="30"/>
+        <v>25</v>
+      </c>
+      <c r="C46" s="29"/>
       <c r="D46" s="26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E46" s="27"/>
-      <c r="F46" s="30">
-        <v>2.62</v>
+      <c r="F46" s="28">
+        <v>3.11</v>
       </c>
       <c r="G46" s="29"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
-      <c r="B47" s="41">
-        <v>4.2600000000000096</v>
-      </c>
-      <c r="C47" s="30"/>
+      <c r="B47" s="23">
+        <v>26</v>
+      </c>
+      <c r="C47" s="29"/>
       <c r="D47" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E47" s="27"/>
-      <c r="F47" s="30">
-        <v>2.62</v>
+      <c r="F47" s="28">
+        <v>3.11</v>
       </c>
       <c r="G47" s="29"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="B48" s="23">
-        <v>4.2700000000000102</v>
-      </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="38" t="s">
-        <v>58</v>
+        <v>27</v>
+      </c>
+      <c r="C48" s="29"/>
+      <c r="D48" s="36" t="s">
+        <v>55</v>
       </c>
       <c r="E48" s="27"/>
-      <c r="F48" s="30">
-        <v>2.62</v>
+      <c r="F48" s="28">
+        <v>3.11</v>
       </c>
       <c r="G48" s="29"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
     </row>
     <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="23">
-        <v>4.28</v>
-      </c>
-      <c r="C49" s="30"/>
-      <c r="D49" s="38" t="s">
-        <v>59</v>
+        <v>28</v>
+      </c>
+      <c r="C49" s="29"/>
+      <c r="D49" s="36" t="s">
+        <v>56</v>
       </c>
       <c r="E49" s="27"/>
-      <c r="F49" s="30">
-        <v>2.62</v>
+      <c r="F49" s="28">
+        <v>3.11</v>
       </c>
       <c r="G49" s="29"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-    </row>
-    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="19">
-        <v>14.5</v>
+      <c r="A50" s="42"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="21"/>
       <c r="D51" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E51" s="22"/>
-      <c r="F51" s="21"/>
+      <c r="F51" s="22"/>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
       <c r="I51" s="21"/>
@@ -2721,212 +2970,212 @@
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="23">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C52" s="30"/>
-      <c r="D52" s="38" t="s">
-        <v>61</v>
+        <v>1</v>
+      </c>
+      <c r="C52" s="29"/>
+      <c r="D52" s="36" t="s">
+        <v>58</v>
       </c>
       <c r="E52" s="27"/>
-      <c r="F52" s="30">
-        <v>2.62</v>
+      <c r="F52" s="28">
+        <v>3.11</v>
       </c>
       <c r="G52" s="29"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="38" t="s">
-        <v>62</v>
+        <v>2</v>
+      </c>
+      <c r="C53" s="29"/>
+      <c r="D53" s="36" t="s">
+        <v>59</v>
       </c>
       <c r="E53" s="27"/>
-      <c r="F53" s="30">
-        <v>2.62</v>
+      <c r="F53" s="28">
+        <v>3.11</v>
       </c>
       <c r="G53" s="29"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="23">
-        <v>5.3</v>
-      </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="49" t="s">
-        <v>63</v>
+        <v>3</v>
+      </c>
+      <c r="C54" s="29"/>
+      <c r="D54" s="46" t="s">
+        <v>60</v>
       </c>
       <c r="E54" s="27"/>
-      <c r="F54" s="30">
-        <v>2.62</v>
+      <c r="F54" s="28">
+        <v>3.11</v>
       </c>
       <c r="G54" s="29"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="23">
-        <v>5.4</v>
-      </c>
-      <c r="C55" s="30"/>
-      <c r="D55" s="38" t="s">
-        <v>64</v>
+        <v>4</v>
+      </c>
+      <c r="C55" s="29"/>
+      <c r="D55" s="36" t="s">
+        <v>61</v>
       </c>
       <c r="E55" s="27"/>
-      <c r="F55" s="30">
-        <v>2.62</v>
+      <c r="F55" s="28">
+        <v>3.11</v>
       </c>
       <c r="G55" s="29"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
     </row>
     <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
       <c r="B56" s="23">
-        <v>5.5</v>
-      </c>
-      <c r="C56" s="30"/>
-      <c r="D56" s="38" t="s">
-        <v>65</v>
+        <v>5</v>
+      </c>
+      <c r="C56" s="29"/>
+      <c r="D56" s="36" t="s">
+        <v>62</v>
       </c>
       <c r="E56" s="27"/>
-      <c r="F56" s="30">
-        <v>2.62</v>
+      <c r="F56" s="28">
+        <v>3.11</v>
       </c>
       <c r="G56" s="29"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="23"/>
       <c r="B57" s="23">
-        <v>5.6</v>
-      </c>
-      <c r="C57" s="30"/>
-      <c r="D57" s="38" t="s">
-        <v>66</v>
+        <v>6</v>
+      </c>
+      <c r="C57" s="29"/>
+      <c r="D57" s="36" t="s">
+        <v>63</v>
       </c>
       <c r="E57" s="27"/>
-      <c r="F57" s="30">
-        <v>2.62</v>
+      <c r="F57" s="28">
+        <v>3.11</v>
       </c>
       <c r="G57" s="29"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="23">
-        <v>5.7</v>
-      </c>
-      <c r="C58" s="30"/>
-      <c r="D58" s="38" t="s">
-        <v>67</v>
+        <v>7</v>
+      </c>
+      <c r="C58" s="29"/>
+      <c r="D58" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="E58" s="27"/>
-      <c r="F58" s="30">
-        <v>2.62</v>
+      <c r="F58" s="28">
+        <v>3.11</v>
       </c>
       <c r="G58" s="29"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="30"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
       <c r="B59" s="23">
-        <v>5.8</v>
-      </c>
-      <c r="C59" s="30"/>
-      <c r="D59" s="38" t="s">
-        <v>68</v>
+        <v>8</v>
+      </c>
+      <c r="C59" s="29"/>
+      <c r="D59" s="36" t="s">
+        <v>65</v>
       </c>
       <c r="E59" s="27"/>
-      <c r="F59" s="30">
-        <v>2.62</v>
+      <c r="F59" s="28">
+        <v>3.11</v>
       </c>
       <c r="G59" s="29"/>
-      <c r="H59" s="30"/>
-      <c r="I59" s="30"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="23">
-        <v>5.9</v>
-      </c>
-      <c r="C60" s="30"/>
-      <c r="D60" s="38" t="s">
-        <v>69</v>
+        <v>9</v>
+      </c>
+      <c r="C60" s="29"/>
+      <c r="D60" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="E60" s="27"/>
-      <c r="F60" s="30">
-        <v>2.62</v>
+      <c r="F60" s="28">
+        <v>3.11</v>
       </c>
       <c r="G60" s="29"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="23"/>
-      <c r="B61" s="41">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C61" s="30"/>
-      <c r="D61" s="40" t="s">
-        <v>70</v>
+      <c r="B61" s="23">
+        <v>10</v>
+      </c>
+      <c r="C61" s="29"/>
+      <c r="D61" s="38" t="s">
+        <v>67</v>
       </c>
       <c r="E61" s="27"/>
-      <c r="F61" s="30">
-        <v>2.62</v>
+      <c r="F61" s="28">
+        <v>3.11</v>
       </c>
       <c r="G61" s="29"/>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
     </row>
     <row r="62" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="23"/>
-      <c r="B62" s="41">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="C62" s="30"/>
-      <c r="D62" s="40" t="s">
-        <v>71</v>
+      <c r="B62" s="23">
+        <v>11</v>
+      </c>
+      <c r="C62" s="29"/>
+      <c r="D62" s="38" t="s">
+        <v>68</v>
       </c>
       <c r="E62" s="27"/>
-      <c r="F62" s="30">
-        <v>2.62</v>
+      <c r="F62" s="28">
+        <v>3.11</v>
       </c>
       <c r="G62" s="29"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-    </row>
-    <row r="64" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="19">
-        <v>14.6</v>
+      <c r="A63" s="30"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="B64" s="20"/>
       <c r="C64" s="21"/>
       <c r="D64" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E64" s="22"/>
-      <c r="F64" s="21"/>
+      <c r="F64" s="22"/>
       <c r="G64" s="21"/>
       <c r="H64" s="21"/>
       <c r="I64" s="21"/>
@@ -2934,110 +3183,110 @@
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="23"/>
       <c r="B65" s="23">
-        <v>6.1</v>
-      </c>
-      <c r="C65" s="30"/>
-      <c r="D65" s="38" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="C65" s="29"/>
+      <c r="D65" s="36" t="s">
+        <v>70</v>
       </c>
       <c r="E65" s="27"/>
-      <c r="F65" s="30">
-        <v>2.62</v>
+      <c r="F65" s="28">
+        <v>3.11</v>
       </c>
       <c r="G65" s="29"/>
-      <c r="H65" s="30"/>
-      <c r="I65" s="30"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
     </row>
     <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="23"/>
       <c r="B66" s="23">
-        <v>6.2</v>
-      </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="38" t="s">
-        <v>74</v>
+        <v>2</v>
+      </c>
+      <c r="C66" s="29"/>
+      <c r="D66" s="36" t="s">
+        <v>71</v>
       </c>
       <c r="E66" s="27"/>
-      <c r="F66" s="30">
-        <v>2.62</v>
+      <c r="F66" s="28">
+        <v>3.11</v>
       </c>
       <c r="G66" s="29"/>
-      <c r="H66" s="30"/>
-      <c r="I66" s="30"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="23"/>
       <c r="B67" s="23">
-        <v>6.3</v>
-      </c>
-      <c r="C67" s="30"/>
-      <c r="D67" s="49" t="s">
-        <v>75</v>
+        <v>3</v>
+      </c>
+      <c r="C67" s="29"/>
+      <c r="D67" s="46" t="s">
+        <v>72</v>
       </c>
       <c r="E67" s="27"/>
-      <c r="F67" s="30">
-        <v>2.62</v>
+      <c r="F67" s="28">
+        <v>3.11</v>
       </c>
       <c r="G67" s="29"/>
-      <c r="H67" s="30"/>
-      <c r="I67" s="30"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="23"/>
       <c r="B68" s="23">
-        <v>6.4</v>
-      </c>
-      <c r="C68" s="30"/>
-      <c r="D68" s="38" t="s">
-        <v>76</v>
+        <v>4</v>
+      </c>
+      <c r="C68" s="29"/>
+      <c r="D68" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="E68" s="27"/>
-      <c r="F68" s="30">
-        <v>2.62</v>
+      <c r="F68" s="28">
+        <v>3.11</v>
       </c>
       <c r="G68" s="29"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
     </row>
     <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="23"/>
       <c r="B69" s="23">
-        <v>6.5</v>
-      </c>
-      <c r="C69" s="30"/>
-      <c r="D69" s="38" t="s">
-        <v>77</v>
+        <v>5</v>
+      </c>
+      <c r="C69" s="29"/>
+      <c r="D69" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="E69" s="27"/>
-      <c r="F69" s="30">
-        <v>2.62</v>
+      <c r="F69" s="28">
+        <v>3.11</v>
       </c>
       <c r="G69" s="29"/>
-      <c r="H69" s="30"/>
-      <c r="I69" s="30"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
-      <c r="B70" s="44"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="45"/>
-      <c r="I70" s="45"/>
-    </row>
-    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A71" s="19">
-        <v>14.7</v>
+      <c r="A70" s="42"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="45"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="B71" s="20"/>
       <c r="C71" s="21"/>
       <c r="D71" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E71" s="22"/>
-      <c r="F71" s="21"/>
+      <c r="F71" s="22"/>
       <c r="G71" s="21"/>
       <c r="H71" s="21"/>
       <c r="I71" s="21"/>
@@ -3045,93 +3294,93 @@
     <row r="72" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="23"/>
       <c r="B72" s="23">
-        <v>7.1</v>
-      </c>
-      <c r="C72" s="30"/>
-      <c r="D72" s="38" t="s">
-        <v>79</v>
+        <v>1</v>
+      </c>
+      <c r="C72" s="29"/>
+      <c r="D72" s="36" t="s">
+        <v>76</v>
       </c>
       <c r="E72" s="27"/>
-      <c r="F72" s="30">
-        <v>2.62</v>
+      <c r="F72" s="28">
+        <v>3.11</v>
       </c>
       <c r="G72" s="29"/>
-      <c r="H72" s="30"/>
-      <c r="I72" s="30"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
     </row>
     <row r="73" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="23"/>
       <c r="B73" s="23">
-        <v>7.2</v>
-      </c>
-      <c r="C73" s="30"/>
-      <c r="D73" s="40" t="s">
-        <v>80</v>
+        <v>2</v>
+      </c>
+      <c r="C73" s="29"/>
+      <c r="D73" s="38" t="s">
+        <v>77</v>
       </c>
       <c r="E73" s="27"/>
-      <c r="F73" s="30">
-        <v>2.62</v>
+      <c r="F73" s="28">
+        <v>3.11</v>
       </c>
       <c r="G73" s="29"/>
-      <c r="H73" s="30"/>
-      <c r="I73" s="30"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
     </row>
     <row r="74" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="23"/>
       <c r="B74" s="23">
-        <v>7.3</v>
-      </c>
-      <c r="C74" s="30"/>
-      <c r="D74" s="40" t="s">
-        <v>81</v>
+        <v>3</v>
+      </c>
+      <c r="C74" s="29"/>
+      <c r="D74" s="38" t="s">
+        <v>78</v>
       </c>
       <c r="E74" s="27"/>
-      <c r="F74" s="30">
-        <v>2.62</v>
+      <c r="F74" s="28">
+        <v>3.11</v>
       </c>
       <c r="G74" s="29"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="30"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
     </row>
     <row r="75" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="23"/>
       <c r="B75" s="23">
-        <v>7.4</v>
-      </c>
-      <c r="C75" s="30"/>
-      <c r="D75" s="38" t="s">
-        <v>82</v>
+        <v>4</v>
+      </c>
+      <c r="C75" s="29"/>
+      <c r="D75" s="36" t="s">
+        <v>79</v>
       </c>
       <c r="E75" s="27"/>
-      <c r="F75" s="30">
-        <v>2.62</v>
+      <c r="F75" s="28">
+        <v>3.11</v>
       </c>
       <c r="G75" s="29"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="48"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="45"/>
-    </row>
-    <row r="77" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="19">
-        <v>14.8</v>
+      <c r="A76" s="42"/>
+      <c r="B76" s="42"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="48"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="43"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="B77" s="20"/>
       <c r="C77" s="21"/>
       <c r="D77" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E77" s="22"/>
-      <c r="F77" s="21"/>
+      <c r="F77" s="22"/>
       <c r="G77" s="21"/>
       <c r="H77" s="21"/>
       <c r="I77" s="21"/>
@@ -3139,195 +3388,195 @@
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="23"/>
       <c r="B78" s="23">
-        <v>8.1</v>
-      </c>
-      <c r="C78" s="30"/>
-      <c r="D78" s="38" t="s">
-        <v>84</v>
+        <v>1</v>
+      </c>
+      <c r="C78" s="29"/>
+      <c r="D78" s="36" t="s">
+        <v>81</v>
       </c>
       <c r="E78" s="27"/>
-      <c r="F78" s="30">
-        <v>2.62</v>
+      <c r="F78" s="28">
+        <v>3.11</v>
       </c>
       <c r="G78" s="29"/>
-      <c r="H78" s="30"/>
-      <c r="I78" s="30"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
     </row>
     <row r="79" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="23"/>
       <c r="B79" s="23">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="C79" s="30"/>
-      <c r="D79" s="38" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="C79" s="29"/>
+      <c r="D79" s="36" t="s">
+        <v>82</v>
       </c>
       <c r="E79" s="27"/>
-      <c r="F79" s="30">
-        <v>2.62</v>
+      <c r="F79" s="28">
+        <v>3.11</v>
       </c>
       <c r="G79" s="29"/>
-      <c r="H79" s="30"/>
-      <c r="I79" s="30"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
     </row>
     <row r="80" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="23"/>
       <c r="B80" s="23">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C80" s="30"/>
-      <c r="D80" s="38" t="s">
-        <v>86</v>
+        <v>3</v>
+      </c>
+      <c r="C80" s="29"/>
+      <c r="D80" s="36" t="s">
+        <v>83</v>
       </c>
       <c r="E80" s="27"/>
-      <c r="F80" s="30">
-        <v>2.62</v>
+      <c r="F80" s="28">
+        <v>3.11</v>
       </c>
       <c r="G80" s="29"/>
-      <c r="H80" s="30"/>
-      <c r="I80" s="30"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
     </row>
     <row r="81" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="B81" s="23">
-        <v>8.4</v>
-      </c>
-      <c r="C81" s="30"/>
-      <c r="D81" s="38" t="s">
-        <v>87</v>
+        <v>4</v>
+      </c>
+      <c r="C81" s="29"/>
+      <c r="D81" s="36" t="s">
+        <v>84</v>
       </c>
       <c r="E81" s="27"/>
-      <c r="F81" s="30">
-        <v>2.62</v>
+      <c r="F81" s="28">
+        <v>3.11</v>
       </c>
       <c r="G81" s="29"/>
-      <c r="H81" s="30"/>
-      <c r="I81" s="30"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
     </row>
     <row r="82" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
       <c r="B82" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="C82" s="30"/>
-      <c r="D82" s="38" t="s">
-        <v>88</v>
+        <v>5</v>
+      </c>
+      <c r="C82" s="29"/>
+      <c r="D82" s="36" t="s">
+        <v>85</v>
       </c>
       <c r="E82" s="27"/>
-      <c r="F82" s="30">
-        <v>2.62</v>
+      <c r="F82" s="28">
+        <v>3.11</v>
       </c>
       <c r="G82" s="29"/>
-      <c r="H82" s="30"/>
-      <c r="I82" s="30"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29"/>
     </row>
     <row r="83" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="23"/>
       <c r="B83" s="23">
-        <v>8.6</v>
-      </c>
-      <c r="C83" s="30"/>
-      <c r="D83" s="38" t="s">
-        <v>89</v>
+        <v>6</v>
+      </c>
+      <c r="C83" s="29"/>
+      <c r="D83" s="36" t="s">
+        <v>86</v>
       </c>
       <c r="E83" s="27"/>
-      <c r="F83" s="30">
-        <v>2.62</v>
+      <c r="F83" s="28">
+        <v>3.11</v>
       </c>
       <c r="G83" s="29"/>
-      <c r="H83" s="30"/>
-      <c r="I83" s="30"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
     </row>
     <row r="84" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="23"/>
       <c r="B84" s="23">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C84" s="30"/>
-      <c r="D84" s="38" t="s">
-        <v>90</v>
+        <v>7</v>
+      </c>
+      <c r="C84" s="29"/>
+      <c r="D84" s="36" t="s">
+        <v>87</v>
       </c>
       <c r="E84" s="27"/>
-      <c r="F84" s="30">
-        <v>2.62</v>
+      <c r="F84" s="28">
+        <v>3.11</v>
       </c>
       <c r="G84" s="29"/>
-      <c r="H84" s="30"/>
-      <c r="I84" s="30"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
     </row>
     <row r="85" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="23"/>
       <c r="B85" s="23">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C85" s="30"/>
-      <c r="D85" s="38" t="s">
-        <v>91</v>
+        <v>8</v>
+      </c>
+      <c r="C85" s="29"/>
+      <c r="D85" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="E85" s="27"/>
-      <c r="F85" s="30">
-        <v>2.62</v>
+      <c r="F85" s="28">
+        <v>3.11</v>
       </c>
       <c r="G85" s="29"/>
-      <c r="H85" s="30"/>
-      <c r="I85" s="30"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
     </row>
     <row r="86" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="23"/>
       <c r="B86" s="23">
-        <v>8.9</v>
-      </c>
-      <c r="C86" s="30"/>
-      <c r="D86" s="38" t="s">
-        <v>92</v>
+        <v>9</v>
+      </c>
+      <c r="C86" s="29"/>
+      <c r="D86" s="36" t="s">
+        <v>89</v>
       </c>
       <c r="E86" s="27"/>
-      <c r="F86" s="30">
-        <v>2.62</v>
+      <c r="F86" s="28">
+        <v>3.11</v>
       </c>
       <c r="G86" s="29"/>
-      <c r="H86" s="30"/>
-      <c r="I86" s="30"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
     </row>
     <row r="87" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A87" s="41"/>
-      <c r="B87" s="41">
-        <v>8.1</v>
-      </c>
-      <c r="C87" s="30"/>
-      <c r="D87" s="38" t="s">
-        <v>93</v>
+      <c r="A87" s="39"/>
+      <c r="B87" s="39">
+        <v>10</v>
+      </c>
+      <c r="C87" s="29"/>
+      <c r="D87" s="36" t="s">
+        <v>90</v>
       </c>
       <c r="E87" s="27"/>
-      <c r="F87" s="30">
-        <v>2.62</v>
+      <c r="F87" s="28">
+        <v>3.11</v>
       </c>
       <c r="G87" s="29"/>
-      <c r="H87" s="30"/>
-      <c r="I87" s="30"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
-      <c r="B88" s="32"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="34"/>
-      <c r="E88" s="35"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="33"/>
-      <c r="I88" s="33"/>
-    </row>
-    <row r="89" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A89" s="19">
-        <v>14.9</v>
+      <c r="A88" s="30"/>
+      <c r="B88" s="31"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="32"/>
+      <c r="I88" s="32"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
+        <v>161</v>
       </c>
       <c r="B89" s="20"/>
       <c r="C89" s="21"/>
       <c r="D89" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E89" s="22"/>
-      <c r="F89" s="21"/>
+      <c r="F89" s="22"/>
       <c r="G89" s="21"/>
       <c r="H89" s="21"/>
       <c r="I89" s="21"/>
@@ -3335,373 +3584,373 @@
     <row r="90" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="23"/>
       <c r="B90" s="23">
-        <v>9.1</v>
-      </c>
-      <c r="C90" s="30"/>
-      <c r="D90" s="38" t="s">
-        <v>95</v>
+        <v>1</v>
+      </c>
+      <c r="C90" s="29"/>
+      <c r="D90" s="36" t="s">
+        <v>92</v>
       </c>
       <c r="E90" s="27"/>
-      <c r="F90" s="30">
-        <v>2.62</v>
+      <c r="F90" s="28">
+        <v>3.11</v>
       </c>
       <c r="G90" s="29"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="23"/>
       <c r="B91" s="23">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C91" s="30"/>
-      <c r="D91" s="38" t="s">
-        <v>96</v>
+        <v>2</v>
+      </c>
+      <c r="C91" s="29"/>
+      <c r="D91" s="36" t="s">
+        <v>93</v>
       </c>
       <c r="E91" s="27"/>
-      <c r="F91" s="30">
-        <v>2.62</v>
+      <c r="F91" s="28">
+        <v>3.11</v>
       </c>
       <c r="G91" s="29"/>
-      <c r="H91" s="30"/>
-      <c r="I91" s="30"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
     </row>
     <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="23"/>
       <c r="B92" s="23">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="C92" s="30"/>
-      <c r="D92" s="38" t="s">
-        <v>97</v>
+        <v>3</v>
+      </c>
+      <c r="C92" s="29"/>
+      <c r="D92" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="E92" s="27"/>
-      <c r="F92" s="30">
-        <v>2.62</v>
+      <c r="F92" s="28">
+        <v>3.11</v>
       </c>
       <c r="G92" s="29"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="30"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
     </row>
     <row r="93" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="23"/>
       <c r="B93" s="23">
-        <v>9.4</v>
-      </c>
-      <c r="C93" s="30"/>
-      <c r="D93" s="38" t="s">
-        <v>98</v>
+        <v>4</v>
+      </c>
+      <c r="C93" s="29"/>
+      <c r="D93" s="36" t="s">
+        <v>95</v>
       </c>
       <c r="E93" s="27"/>
-      <c r="F93" s="30">
-        <v>2.62</v>
+      <c r="F93" s="28">
+        <v>3.11</v>
       </c>
       <c r="G93" s="29"/>
-      <c r="H93" s="30"/>
-      <c r="I93" s="30"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="29"/>
     </row>
     <row r="94" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="23"/>
       <c r="B94" s="23">
-        <v>9.5</v>
-      </c>
-      <c r="C94" s="30"/>
-      <c r="D94" s="38" t="s">
-        <v>99</v>
+        <v>5</v>
+      </c>
+      <c r="C94" s="29"/>
+      <c r="D94" s="36" t="s">
+        <v>96</v>
       </c>
       <c r="E94" s="27"/>
-      <c r="F94" s="30">
-        <v>2.62</v>
+      <c r="F94" s="28">
+        <v>3.11</v>
       </c>
       <c r="G94" s="29"/>
-      <c r="H94" s="30"/>
-      <c r="I94" s="30"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="29"/>
     </row>
     <row r="95" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="23"/>
       <c r="B95" s="23">
-        <v>9.6</v>
-      </c>
-      <c r="C95" s="30"/>
-      <c r="D95" s="38" t="s">
-        <v>100</v>
+        <v>6</v>
+      </c>
+      <c r="C95" s="29"/>
+      <c r="D95" s="36" t="s">
+        <v>97</v>
       </c>
       <c r="E95" s="27"/>
-      <c r="F95" s="30">
-        <v>2.62</v>
+      <c r="F95" s="28">
+        <v>3.11</v>
       </c>
       <c r="G95" s="29"/>
-      <c r="H95" s="30"/>
-      <c r="I95" s="30"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="29"/>
     </row>
     <row r="96" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="23"/>
       <c r="B96" s="23">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="C96" s="30"/>
-      <c r="D96" s="38" t="s">
-        <v>101</v>
+        <v>7</v>
+      </c>
+      <c r="C96" s="29"/>
+      <c r="D96" s="36" t="s">
+        <v>98</v>
       </c>
       <c r="E96" s="27"/>
-      <c r="F96" s="30">
-        <v>2.62</v>
+      <c r="F96" s="28">
+        <v>3.11</v>
       </c>
       <c r="G96" s="29"/>
-      <c r="H96" s="30"/>
-      <c r="I96" s="30"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
     </row>
     <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="23"/>
       <c r="B97" s="23">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="C97" s="30"/>
-      <c r="D97" s="38" t="s">
-        <v>102</v>
+        <v>8</v>
+      </c>
+      <c r="C97" s="29"/>
+      <c r="D97" s="36" t="s">
+        <v>99</v>
       </c>
       <c r="E97" s="27"/>
-      <c r="F97" s="30">
-        <v>2.62</v>
+      <c r="F97" s="28">
+        <v>3.11</v>
       </c>
       <c r="G97" s="29"/>
-      <c r="H97" s="30"/>
-      <c r="I97" s="30"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
     </row>
     <row r="98" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="23"/>
       <c r="B98" s="23">
-        <v>9.9</v>
-      </c>
-      <c r="C98" s="30"/>
-      <c r="D98" s="38" t="s">
-        <v>103</v>
+        <v>9</v>
+      </c>
+      <c r="C98" s="29"/>
+      <c r="D98" s="36" t="s">
+        <v>100</v>
       </c>
       <c r="E98" s="27"/>
-      <c r="F98" s="30">
-        <v>2.62</v>
+      <c r="F98" s="28">
+        <v>3.11</v>
       </c>
       <c r="G98" s="29"/>
-      <c r="H98" s="30"/>
-      <c r="I98" s="30"/>
+      <c r="H98" s="29"/>
+      <c r="I98" s="29"/>
     </row>
     <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="23"/>
-      <c r="B99" s="41">
-        <v>9.1</v>
-      </c>
-      <c r="C99" s="30"/>
-      <c r="D99" s="38" t="s">
-        <v>104</v>
+      <c r="B99" s="23">
+        <v>10</v>
+      </c>
+      <c r="C99" s="29"/>
+      <c r="D99" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="E99" s="27"/>
-      <c r="F99" s="30">
-        <v>2.62</v>
+      <c r="F99" s="28">
+        <v>3.11</v>
       </c>
       <c r="G99" s="29"/>
-      <c r="H99" s="30"/>
-      <c r="I99" s="30"/>
+      <c r="H99" s="29"/>
+      <c r="I99" s="29"/>
     </row>
     <row r="100" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="23"/>
       <c r="B100" s="23">
-        <v>9.11</v>
-      </c>
-      <c r="C100" s="30"/>
-      <c r="D100" s="38" t="s">
-        <v>105</v>
+        <v>11</v>
+      </c>
+      <c r="C100" s="29"/>
+      <c r="D100" s="36" t="s">
+        <v>102</v>
       </c>
       <c r="E100" s="27"/>
-      <c r="F100" s="30">
-        <v>2.62</v>
+      <c r="F100" s="28">
+        <v>3.11</v>
       </c>
       <c r="G100" s="29"/>
-      <c r="H100" s="30"/>
-      <c r="I100" s="30"/>
+      <c r="H100" s="29"/>
+      <c r="I100" s="29"/>
     </row>
     <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="23"/>
       <c r="B101" s="23">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="C101" s="30"/>
-      <c r="D101" s="38" t="s">
-        <v>106</v>
+        <v>12</v>
+      </c>
+      <c r="C101" s="29"/>
+      <c r="D101" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="E101" s="27"/>
-      <c r="F101" s="30">
-        <v>2.62</v>
+      <c r="F101" s="28">
+        <v>3.11</v>
       </c>
       <c r="G101" s="29"/>
-      <c r="H101" s="30"/>
-      <c r="I101" s="30"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
     </row>
     <row r="102" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="23"/>
-      <c r="B102" s="41">
-        <v>9.1300000000000008</v>
-      </c>
-      <c r="C102" s="30"/>
-      <c r="D102" s="38" t="s">
-        <v>107</v>
+      <c r="B102" s="23">
+        <v>13</v>
+      </c>
+      <c r="C102" s="29"/>
+      <c r="D102" s="36" t="s">
+        <v>104</v>
       </c>
       <c r="E102" s="27"/>
-      <c r="F102" s="30">
-        <v>2.62</v>
+      <c r="F102" s="28">
+        <v>3.11</v>
       </c>
       <c r="G102" s="29"/>
-      <c r="H102" s="30"/>
-      <c r="I102" s="30"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="29"/>
     </row>
     <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="23"/>
       <c r="B103" s="23">
-        <v>9.14</v>
-      </c>
-      <c r="C103" s="30"/>
-      <c r="D103" s="38" t="s">
-        <v>108</v>
+        <v>14</v>
+      </c>
+      <c r="C103" s="29"/>
+      <c r="D103" s="36" t="s">
+        <v>105</v>
       </c>
       <c r="E103" s="27"/>
-      <c r="F103" s="30">
-        <v>2.62</v>
+      <c r="F103" s="28">
+        <v>3.11</v>
       </c>
       <c r="G103" s="29"/>
-      <c r="H103" s="30"/>
-      <c r="I103" s="30"/>
+      <c r="H103" s="29"/>
+      <c r="I103" s="29"/>
     </row>
     <row r="104" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="41"/>
-      <c r="B104" s="41">
-        <v>9.15</v>
-      </c>
-      <c r="C104" s="30"/>
-      <c r="D104" s="38" t="s">
-        <v>109</v>
+      <c r="A104" s="39"/>
+      <c r="B104" s="23">
+        <v>15</v>
+      </c>
+      <c r="C104" s="29"/>
+      <c r="D104" s="36" t="s">
+        <v>106</v>
       </c>
       <c r="E104" s="27"/>
-      <c r="F104" s="30">
-        <v>2.62</v>
+      <c r="F104" s="28">
+        <v>3.11</v>
       </c>
       <c r="G104" s="29"/>
-      <c r="H104" s="30"/>
-      <c r="I104" s="30"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="29"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="23"/>
       <c r="B105" s="23">
-        <v>9.16</v>
-      </c>
-      <c r="C105" s="30"/>
-      <c r="D105" s="38" t="s">
-        <v>110</v>
+        <v>16</v>
+      </c>
+      <c r="C105" s="29"/>
+      <c r="D105" s="36" t="s">
+        <v>107</v>
       </c>
       <c r="E105" s="27"/>
-      <c r="F105" s="30">
-        <v>2.62</v>
+      <c r="F105" s="28">
+        <v>3.11</v>
       </c>
       <c r="G105" s="29"/>
-      <c r="H105" s="30"/>
-      <c r="I105" s="30"/>
+      <c r="H105" s="29"/>
+      <c r="I105" s="29"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="23"/>
-      <c r="B106" s="41">
-        <v>9.17</v>
-      </c>
-      <c r="C106" s="30"/>
-      <c r="D106" s="38" t="s">
-        <v>111</v>
+      <c r="B106" s="23">
+        <v>17</v>
+      </c>
+      <c r="C106" s="29"/>
+      <c r="D106" s="36" t="s">
+        <v>108</v>
       </c>
       <c r="E106" s="27"/>
-      <c r="F106" s="30">
-        <v>2.62</v>
+      <c r="F106" s="28">
+        <v>3.11</v>
       </c>
       <c r="G106" s="29"/>
-      <c r="H106" s="30"/>
-      <c r="I106" s="30"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
     </row>
     <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="23"/>
       <c r="B107" s="23">
-        <v>9.18</v>
-      </c>
-      <c r="C107" s="30"/>
-      <c r="D107" s="38" t="s">
-        <v>112</v>
+        <v>18</v>
+      </c>
+      <c r="C107" s="29"/>
+      <c r="D107" s="36" t="s">
+        <v>109</v>
       </c>
       <c r="E107" s="27"/>
-      <c r="F107" s="30">
-        <v>2.62</v>
+      <c r="F107" s="28">
+        <v>3.11</v>
       </c>
       <c r="G107" s="29"/>
-      <c r="H107" s="30"/>
-      <c r="I107" s="30"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="23"/>
-      <c r="B108" s="41">
-        <v>9.19</v>
-      </c>
-      <c r="C108" s="30"/>
-      <c r="D108" s="38" t="s">
-        <v>113</v>
+      <c r="B108" s="23">
+        <v>19</v>
+      </c>
+      <c r="C108" s="29"/>
+      <c r="D108" s="36" t="s">
+        <v>110</v>
       </c>
       <c r="E108" s="27"/>
-      <c r="F108" s="30">
-        <v>2.62</v>
+      <c r="F108" s="28">
+        <v>3.11</v>
       </c>
       <c r="G108" s="29"/>
-      <c r="H108" s="30"/>
-      <c r="I108" s="30"/>
+      <c r="H108" s="29"/>
+      <c r="I108" s="29"/>
     </row>
     <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="23"/>
-      <c r="B109" s="41">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C109" s="30"/>
-      <c r="D109" s="38" t="s">
-        <v>114</v>
+      <c r="B109" s="23">
+        <v>20</v>
+      </c>
+      <c r="C109" s="29"/>
+      <c r="D109" s="36" t="s">
+        <v>111</v>
       </c>
       <c r="E109" s="27"/>
-      <c r="F109" s="30">
-        <v>2.62</v>
+      <c r="F109" s="28">
+        <v>3.11</v>
       </c>
       <c r="G109" s="29"/>
-      <c r="H109" s="30"/>
-      <c r="I109" s="30"/>
+      <c r="H109" s="29"/>
+      <c r="I109" s="29"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="31"/>
-      <c r="B110" s="32"/>
-      <c r="C110" s="33"/>
-      <c r="D110" s="34"/>
-      <c r="E110" s="36"/>
-      <c r="F110" s="33"/>
-      <c r="G110" s="36"/>
-      <c r="H110" s="33"/>
-      <c r="I110" s="33"/>
+      <c r="A110" s="30"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="32"/>
+      <c r="D110" s="33"/>
+      <c r="E110" s="35"/>
+      <c r="F110" s="28"/>
+      <c r="G110" s="29"/>
+      <c r="H110" s="32"/>
+      <c r="I110" s="32"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="31"/>
-      <c r="B111" s="32"/>
-      <c r="C111" s="33"/>
-      <c r="D111" s="34"/>
-      <c r="E111" s="36"/>
-      <c r="F111" s="33"/>
-      <c r="G111" s="36"/>
-      <c r="H111" s="33"/>
-      <c r="I111" s="33"/>
-    </row>
-    <row r="112" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A112" s="52">
-        <v>14.1</v>
+      <c r="A111" s="30"/>
+      <c r="B111" s="31"/>
+      <c r="C111" s="32"/>
+      <c r="D111" s="33"/>
+      <c r="E111" s="35"/>
+      <c r="F111" s="28"/>
+      <c r="G111" s="29"/>
+      <c r="H111" s="32"/>
+      <c r="I111" s="32"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="49">
+        <v>6.4</v>
       </c>
       <c r="B112" s="20"/>
       <c r="C112" s="21"/>
       <c r="D112" s="19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E112" s="22"/>
       <c r="F112" s="22"/>
@@ -3712,90 +3961,90 @@
     <row r="113" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" s="23"/>
       <c r="B113" s="23">
-        <v>10.1</v>
-      </c>
-      <c r="C113" s="30"/>
-      <c r="D113" s="38" t="s">
-        <v>116</v>
+        <v>1</v>
+      </c>
+      <c r="C113" s="29"/>
+      <c r="D113" s="36" t="s">
+        <v>113</v>
       </c>
       <c r="E113" s="27"/>
-      <c r="F113" s="30">
-        <v>2.62</v>
+      <c r="F113" s="28">
+        <v>3.11</v>
       </c>
       <c r="G113" s="29"/>
-      <c r="H113" s="30"/>
-      <c r="I113" s="30"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
     </row>
     <row r="114" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A114" s="23"/>
       <c r="B114" s="23">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="C114" s="30"/>
-      <c r="D114" s="38" t="s">
-        <v>117</v>
+        <v>2</v>
+      </c>
+      <c r="C114" s="29"/>
+      <c r="D114" s="36" t="s">
+        <v>114</v>
       </c>
       <c r="E114" s="27"/>
-      <c r="F114" s="30">
-        <v>2.62</v>
+      <c r="F114" s="28">
+        <v>3.11</v>
       </c>
       <c r="G114" s="29"/>
-      <c r="H114" s="30"/>
-      <c r="I114" s="30"/>
+      <c r="H114" s="29"/>
+      <c r="I114" s="29"/>
     </row>
     <row r="115" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="23"/>
       <c r="B115" s="23">
-        <v>10.3</v>
-      </c>
-      <c r="C115" s="30"/>
-      <c r="D115" s="38" t="s">
-        <v>118</v>
+        <v>3</v>
+      </c>
+      <c r="C115" s="29"/>
+      <c r="D115" s="36" t="s">
+        <v>115</v>
       </c>
       <c r="E115" s="27"/>
-      <c r="F115" s="30">
-        <v>2.62</v>
+      <c r="F115" s="28">
+        <v>3.11</v>
       </c>
       <c r="G115" s="29"/>
-      <c r="H115" s="30"/>
-      <c r="I115" s="30"/>
+      <c r="H115" s="29"/>
+      <c r="I115" s="29"/>
     </row>
     <row r="116" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="23"/>
       <c r="B116" s="23">
-        <v>10.4</v>
-      </c>
-      <c r="C116" s="30"/>
-      <c r="D116" s="38" t="s">
-        <v>119</v>
+        <v>4</v>
+      </c>
+      <c r="C116" s="29"/>
+      <c r="D116" s="36" t="s">
+        <v>116</v>
       </c>
       <c r="E116" s="27"/>
-      <c r="F116" s="30">
-        <v>2.62</v>
+      <c r="F116" s="28">
+        <v>3.11</v>
       </c>
       <c r="G116" s="29"/>
-      <c r="H116" s="30"/>
-      <c r="I116" s="30"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="29"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
-      <c r="B117" s="32"/>
-      <c r="C117" s="33"/>
-      <c r="D117" s="34"/>
-      <c r="E117" s="35"/>
-      <c r="F117" s="30"/>
-      <c r="G117" s="36"/>
-      <c r="H117" s="33"/>
-      <c r="I117" s="33"/>
-    </row>
-    <row r="118" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A117" s="30"/>
+      <c r="B117" s="31"/>
+      <c r="C117" s="32"/>
+      <c r="D117" s="33"/>
+      <c r="E117" s="34"/>
+      <c r="F117" s="28"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="32"/>
+      <c r="I117" s="32"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="19" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B118" s="20"/>
       <c r="C118" s="21"/>
       <c r="D118" s="19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E118" s="22"/>
       <c r="F118" s="22"/>
@@ -3806,107 +4055,107 @@
     <row r="119" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="23"/>
       <c r="B119" s="23">
-        <v>11.1</v>
-      </c>
-      <c r="C119" s="30"/>
-      <c r="D119" s="38" t="s">
-        <v>122</v>
+        <v>1</v>
+      </c>
+      <c r="C119" s="29"/>
+      <c r="D119" s="36" t="s">
+        <v>118</v>
       </c>
       <c r="E119" s="27"/>
-      <c r="F119" s="30">
-        <v>2.62</v>
+      <c r="F119" s="28">
+        <v>3.11</v>
       </c>
       <c r="G119" s="29"/>
-      <c r="H119" s="30"/>
-      <c r="I119" s="30"/>
+      <c r="H119" s="29"/>
+      <c r="I119" s="29"/>
     </row>
     <row r="120" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A120" s="23"/>
       <c r="B120" s="23">
-        <v>11.2</v>
-      </c>
-      <c r="C120" s="30"/>
-      <c r="D120" s="38" t="s">
-        <v>123</v>
+        <v>2</v>
+      </c>
+      <c r="C120" s="29"/>
+      <c r="D120" s="36" t="s">
+        <v>119</v>
       </c>
       <c r="E120" s="27"/>
-      <c r="F120" s="30">
-        <v>2.62</v>
+      <c r="F120" s="28">
+        <v>3.11</v>
       </c>
       <c r="G120" s="29"/>
-      <c r="H120" s="30"/>
-      <c r="I120" s="30"/>
+      <c r="H120" s="29"/>
+      <c r="I120" s="29"/>
     </row>
     <row r="121" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="23"/>
       <c r="B121" s="23">
-        <v>11.3</v>
-      </c>
-      <c r="C121" s="30"/>
-      <c r="D121" s="38" t="s">
-        <v>124</v>
+        <v>3</v>
+      </c>
+      <c r="C121" s="29"/>
+      <c r="D121" s="36" t="s">
+        <v>120</v>
       </c>
       <c r="E121" s="27"/>
-      <c r="F121" s="30">
-        <v>2.62</v>
+      <c r="F121" s="28">
+        <v>3.11</v>
       </c>
       <c r="G121" s="29"/>
-      <c r="H121" s="30"/>
-      <c r="I121" s="30"/>
+      <c r="H121" s="29"/>
+      <c r="I121" s="29"/>
     </row>
     <row r="122" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="23"/>
       <c r="B122" s="23">
-        <v>11.4</v>
-      </c>
-      <c r="C122" s="30"/>
-      <c r="D122" s="38" t="s">
-        <v>125</v>
+        <v>4</v>
+      </c>
+      <c r="C122" s="29"/>
+      <c r="D122" s="36" t="s">
+        <v>121</v>
       </c>
       <c r="E122" s="27"/>
-      <c r="F122" s="30">
-        <v>2.62</v>
+      <c r="F122" s="28">
+        <v>3.11</v>
       </c>
       <c r="G122" s="29"/>
-      <c r="H122" s="30"/>
-      <c r="I122" s="30"/>
+      <c r="H122" s="29"/>
+      <c r="I122" s="29"/>
     </row>
     <row r="123" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="23"/>
       <c r="B123" s="23">
-        <v>11.5</v>
-      </c>
-      <c r="C123" s="30"/>
-      <c r="D123" s="38" t="s">
-        <v>126</v>
+        <v>5</v>
+      </c>
+      <c r="C123" s="29"/>
+      <c r="D123" s="36" t="s">
+        <v>122</v>
       </c>
       <c r="E123" s="27"/>
-      <c r="F123" s="30">
-        <v>2.62</v>
+      <c r="F123" s="28">
+        <v>3.11</v>
       </c>
       <c r="G123" s="29"/>
-      <c r="H123" s="30"/>
-      <c r="I123" s="30"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="44"/>
-      <c r="B124" s="53"/>
-      <c r="C124" s="33"/>
-      <c r="D124" s="51"/>
-      <c r="E124" s="54"/>
-      <c r="F124" s="30"/>
-      <c r="G124" s="36"/>
-      <c r="H124" s="33"/>
-      <c r="I124" s="33"/>
-    </row>
-    <row r="125" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A124" s="42"/>
+      <c r="B124" s="50"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="48"/>
+      <c r="E124" s="51"/>
+      <c r="F124" s="28"/>
+      <c r="G124" s="29"/>
+      <c r="H124" s="32"/>
+      <c r="I124" s="32"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="19" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="B125" s="20"/>
       <c r="C125" s="21"/>
       <c r="D125" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E125" s="22"/>
       <c r="F125" s="22"/>
@@ -3917,124 +4166,124 @@
     <row r="126" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" s="23"/>
       <c r="B126" s="23">
-        <v>12.1</v>
-      </c>
-      <c r="C126" s="30"/>
-      <c r="D126" s="38" t="s">
-        <v>129</v>
+        <v>1</v>
+      </c>
+      <c r="C126" s="29"/>
+      <c r="D126" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="E126" s="27"/>
-      <c r="F126" s="30">
-        <v>2.62</v>
+      <c r="F126" s="28">
+        <v>3.11</v>
       </c>
       <c r="G126" s="29"/>
-      <c r="H126" s="30"/>
-      <c r="I126" s="30"/>
+      <c r="H126" s="29"/>
+      <c r="I126" s="29"/>
     </row>
     <row r="127" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="23"/>
       <c r="B127" s="23">
-        <v>12.2</v>
-      </c>
-      <c r="C127" s="30"/>
-      <c r="D127" s="38" t="s">
-        <v>130</v>
+        <v>2</v>
+      </c>
+      <c r="C127" s="29"/>
+      <c r="D127" s="36" t="s">
+        <v>125</v>
       </c>
       <c r="E127" s="27"/>
-      <c r="F127" s="30">
-        <v>2.62</v>
+      <c r="F127" s="28">
+        <v>3.11</v>
       </c>
       <c r="G127" s="29"/>
-      <c r="H127" s="30"/>
-      <c r="I127" s="30"/>
+      <c r="H127" s="29"/>
+      <c r="I127" s="29"/>
     </row>
     <row r="128" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" s="23"/>
       <c r="B128" s="23">
-        <v>12.3</v>
-      </c>
-      <c r="C128" s="30"/>
-      <c r="D128" s="38" t="s">
-        <v>131</v>
+        <v>3</v>
+      </c>
+      <c r="C128" s="29"/>
+      <c r="D128" s="36" t="s">
+        <v>126</v>
       </c>
       <c r="E128" s="27"/>
-      <c r="F128" s="30">
-        <v>2.62</v>
+      <c r="F128" s="28">
+        <v>3.11</v>
       </c>
       <c r="G128" s="29"/>
-      <c r="H128" s="30"/>
-      <c r="I128" s="30"/>
+      <c r="H128" s="29"/>
+      <c r="I128" s="29"/>
     </row>
     <row r="129" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="23"/>
       <c r="B129" s="23">
-        <v>12.4</v>
-      </c>
-      <c r="C129" s="30"/>
-      <c r="D129" s="38" t="s">
-        <v>132</v>
+        <v>4</v>
+      </c>
+      <c r="C129" s="29"/>
+      <c r="D129" s="36" t="s">
+        <v>127</v>
       </c>
       <c r="E129" s="27"/>
-      <c r="F129" s="30">
-        <v>2.62</v>
+      <c r="F129" s="28">
+        <v>3.11</v>
       </c>
       <c r="G129" s="29"/>
-      <c r="H129" s="30"/>
-      <c r="I129" s="30"/>
+      <c r="H129" s="29"/>
+      <c r="I129" s="29"/>
     </row>
     <row r="130" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="23"/>
       <c r="B130" s="23">
-        <v>12.5</v>
-      </c>
-      <c r="C130" s="30"/>
-      <c r="D130" s="38" t="s">
-        <v>133</v>
+        <v>5</v>
+      </c>
+      <c r="C130" s="29"/>
+      <c r="D130" s="36" t="s">
+        <v>128</v>
       </c>
       <c r="E130" s="27"/>
-      <c r="F130" s="30">
-        <v>2.62</v>
+      <c r="F130" s="28">
+        <v>3.11</v>
       </c>
       <c r="G130" s="29"/>
-      <c r="H130" s="30"/>
-      <c r="I130" s="30"/>
+      <c r="H130" s="29"/>
+      <c r="I130" s="29"/>
     </row>
     <row r="131" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="23"/>
       <c r="B131" s="23">
-        <v>12.6</v>
-      </c>
-      <c r="C131" s="30"/>
-      <c r="D131" s="38" t="s">
-        <v>134</v>
+        <v>6</v>
+      </c>
+      <c r="C131" s="29"/>
+      <c r="D131" s="36" t="s">
+        <v>129</v>
       </c>
       <c r="E131" s="27"/>
-      <c r="F131" s="30">
-        <v>2.62</v>
+      <c r="F131" s="28">
+        <v>3.11</v>
       </c>
       <c r="G131" s="29"/>
-      <c r="H131" s="30"/>
-      <c r="I131" s="30"/>
+      <c r="H131" s="29"/>
+      <c r="I131" s="29"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="39"/>
-      <c r="B132" s="32"/>
-      <c r="C132" s="33"/>
-      <c r="D132" s="34"/>
-      <c r="E132" s="35"/>
-      <c r="F132" s="30"/>
-      <c r="G132" s="36"/>
-      <c r="H132" s="33"/>
-      <c r="I132" s="33"/>
-    </row>
-    <row r="133" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A132" s="37"/>
+      <c r="B132" s="31"/>
+      <c r="C132" s="32"/>
+      <c r="D132" s="33"/>
+      <c r="E132" s="34"/>
+      <c r="F132" s="28"/>
+      <c r="G132" s="29"/>
+      <c r="H132" s="32"/>
+      <c r="I132" s="32"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="19" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="B133" s="20"/>
       <c r="C133" s="21"/>
       <c r="D133" s="19" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E133" s="22"/>
       <c r="F133" s="22"/>
@@ -4045,209 +4294,209 @@
     <row r="134" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="23"/>
       <c r="B134" s="23">
-        <v>13.1</v>
-      </c>
-      <c r="C134" s="30"/>
-      <c r="D134" s="38" t="s">
-        <v>137</v>
+        <v>1</v>
+      </c>
+      <c r="C134" s="29"/>
+      <c r="D134" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="E134" s="27"/>
-      <c r="F134" s="30">
-        <v>2.62</v>
+      <c r="F134" s="28">
+        <v>3.11</v>
       </c>
       <c r="G134" s="29"/>
-      <c r="H134" s="30"/>
-      <c r="I134" s="30"/>
+      <c r="H134" s="29"/>
+      <c r="I134" s="29"/>
     </row>
     <row r="135" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="23"/>
       <c r="B135" s="23">
-        <v>13.2</v>
-      </c>
-      <c r="C135" s="30"/>
-      <c r="D135" s="38" t="s">
-        <v>138</v>
+        <v>2</v>
+      </c>
+      <c r="C135" s="29"/>
+      <c r="D135" s="36" t="s">
+        <v>132</v>
       </c>
       <c r="E135" s="27"/>
-      <c r="F135" s="30">
-        <v>2.62</v>
+      <c r="F135" s="28">
+        <v>3.11</v>
       </c>
       <c r="G135" s="29"/>
-      <c r="H135" s="30"/>
-      <c r="I135" s="30"/>
+      <c r="H135" s="29"/>
+      <c r="I135" s="29"/>
     </row>
     <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="23"/>
       <c r="B136" s="23">
-        <v>13.3</v>
-      </c>
-      <c r="C136" s="30"/>
-      <c r="D136" s="38" t="s">
-        <v>139</v>
+        <v>3</v>
+      </c>
+      <c r="C136" s="29"/>
+      <c r="D136" s="36" t="s">
+        <v>133</v>
       </c>
       <c r="E136" s="27"/>
-      <c r="F136" s="30">
-        <v>2.62</v>
+      <c r="F136" s="28">
+        <v>3.11</v>
       </c>
       <c r="G136" s="29"/>
-      <c r="H136" s="30"/>
-      <c r="I136" s="30"/>
+      <c r="H136" s="29"/>
+      <c r="I136" s="29"/>
     </row>
     <row r="137" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="23"/>
       <c r="B137" s="23">
-        <v>13.4</v>
-      </c>
-      <c r="C137" s="30"/>
-      <c r="D137" s="38" t="s">
-        <v>140</v>
+        <v>4</v>
+      </c>
+      <c r="C137" s="29"/>
+      <c r="D137" s="36" t="s">
+        <v>134</v>
       </c>
       <c r="E137" s="27"/>
-      <c r="F137" s="30">
-        <v>2.62</v>
+      <c r="F137" s="28">
+        <v>3.11</v>
       </c>
       <c r="G137" s="29"/>
-      <c r="H137" s="30"/>
-      <c r="I137" s="30"/>
+      <c r="H137" s="29"/>
+      <c r="I137" s="29"/>
     </row>
     <row r="138" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="23"/>
       <c r="B138" s="23">
-        <v>13.5</v>
-      </c>
-      <c r="C138" s="30"/>
-      <c r="D138" s="38" t="s">
-        <v>141</v>
+        <v>5</v>
+      </c>
+      <c r="C138" s="29"/>
+      <c r="D138" s="36" t="s">
+        <v>135</v>
       </c>
       <c r="E138" s="27"/>
-      <c r="F138" s="30">
-        <v>2.62</v>
+      <c r="F138" s="28">
+        <v>3.11</v>
       </c>
       <c r="G138" s="29"/>
-      <c r="H138" s="30"/>
-      <c r="I138" s="30"/>
+      <c r="H138" s="29"/>
+      <c r="I138" s="29"/>
     </row>
     <row r="139" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" s="23"/>
       <c r="B139" s="23">
-        <v>13.6</v>
-      </c>
-      <c r="C139" s="30"/>
-      <c r="D139" s="38" t="s">
-        <v>142</v>
+        <v>6</v>
+      </c>
+      <c r="C139" s="29"/>
+      <c r="D139" s="36" t="s">
+        <v>136</v>
       </c>
       <c r="E139" s="27"/>
-      <c r="F139" s="30">
-        <v>2.62</v>
+      <c r="F139" s="28">
+        <v>3.11</v>
       </c>
       <c r="G139" s="29"/>
-      <c r="H139" s="30"/>
-      <c r="I139" s="30"/>
+      <c r="H139" s="29"/>
+      <c r="I139" s="29"/>
     </row>
     <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="23"/>
       <c r="B140" s="23">
-        <v>13.7</v>
-      </c>
-      <c r="C140" s="30"/>
-      <c r="D140" s="38" t="s">
-        <v>143</v>
+        <v>7</v>
+      </c>
+      <c r="C140" s="29"/>
+      <c r="D140" s="36" t="s">
+        <v>137</v>
       </c>
       <c r="E140" s="27"/>
-      <c r="F140" s="30">
-        <v>2.62</v>
+      <c r="F140" s="28">
+        <v>3.11</v>
       </c>
       <c r="G140" s="29"/>
-      <c r="H140" s="30"/>
-      <c r="I140" s="30"/>
+      <c r="H140" s="29"/>
+      <c r="I140" s="29"/>
     </row>
     <row r="141" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A141" s="23"/>
       <c r="B141" s="23">
-        <v>13.8</v>
-      </c>
-      <c r="C141" s="30"/>
-      <c r="D141" s="38" t="s">
-        <v>144</v>
+        <v>8</v>
+      </c>
+      <c r="C141" s="29"/>
+      <c r="D141" s="36" t="s">
+        <v>138</v>
       </c>
       <c r="E141" s="27"/>
-      <c r="F141" s="30">
-        <v>2.62</v>
+      <c r="F141" s="28">
+        <v>3.11</v>
       </c>
       <c r="G141" s="29"/>
-      <c r="H141" s="30"/>
-      <c r="I141" s="30"/>
+      <c r="H141" s="29"/>
+      <c r="I141" s="29"/>
     </row>
     <row r="142" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="23"/>
       <c r="B142" s="23">
-        <v>13.9</v>
-      </c>
-      <c r="C142" s="30"/>
-      <c r="D142" s="38" t="s">
-        <v>145</v>
+        <v>9</v>
+      </c>
+      <c r="C142" s="29"/>
+      <c r="D142" s="36" t="s">
+        <v>139</v>
       </c>
       <c r="E142" s="27"/>
-      <c r="F142" s="30">
-        <v>2.62</v>
+      <c r="F142" s="28">
+        <v>3.11</v>
       </c>
       <c r="G142" s="29"/>
-      <c r="H142" s="30"/>
-      <c r="I142" s="30"/>
+      <c r="H142" s="29"/>
+      <c r="I142" s="29"/>
     </row>
     <row r="143" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A143" s="23"/>
-      <c r="B143" s="41">
-        <v>13.1</v>
-      </c>
-      <c r="C143" s="30"/>
-      <c r="D143" s="38" t="s">
-        <v>146</v>
+      <c r="B143" s="23">
+        <v>10</v>
+      </c>
+      <c r="C143" s="29"/>
+      <c r="D143" s="36" t="s">
+        <v>140</v>
       </c>
       <c r="E143" s="27"/>
-      <c r="F143" s="30">
-        <v>2.62</v>
+      <c r="F143" s="28">
+        <v>3.11</v>
       </c>
       <c r="G143" s="29"/>
-      <c r="H143" s="30"/>
-      <c r="I143" s="30"/>
+      <c r="H143" s="29"/>
+      <c r="I143" s="29"/>
     </row>
     <row r="144" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="23"/>
       <c r="B144" s="23">
-        <v>13.11</v>
-      </c>
-      <c r="C144" s="30"/>
-      <c r="D144" s="38" t="s">
-        <v>147</v>
+        <v>11</v>
+      </c>
+      <c r="C144" s="29"/>
+      <c r="D144" s="36" t="s">
+        <v>141</v>
       </c>
       <c r="E144" s="27"/>
-      <c r="F144" s="30">
-        <v>2.62</v>
+      <c r="F144" s="28">
+        <v>3.11</v>
       </c>
       <c r="G144" s="29"/>
-      <c r="H144" s="30"/>
-      <c r="I144" s="30"/>
+      <c r="H144" s="29"/>
+      <c r="I144" s="29"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="31"/>
-      <c r="B145" s="32"/>
-      <c r="C145" s="33"/>
-      <c r="D145" s="34"/>
-      <c r="E145" s="35"/>
-      <c r="F145" s="30"/>
-      <c r="G145" s="36"/>
-      <c r="H145" s="33"/>
-      <c r="I145" s="33"/>
-    </row>
-    <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="30"/>
+      <c r="B145" s="31"/>
+      <c r="C145" s="32"/>
+      <c r="D145" s="33"/>
+      <c r="E145" s="34"/>
+      <c r="F145" s="28"/>
+      <c r="G145" s="29"/>
+      <c r="H145" s="32"/>
+      <c r="I145" s="32"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="19">
         <v>6.6</v>
       </c>
       <c r="B146" s="20"/>
       <c r="C146" s="21"/>
       <c r="D146" s="19" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E146" s="22"/>
       <c r="F146" s="22"/>
@@ -4260,421 +4509,205 @@
       <c r="B147" s="23">
         <v>14.1</v>
       </c>
-      <c r="C147" s="30"/>
-      <c r="D147" s="38" t="s">
-        <v>149</v>
+      <c r="C147" s="29"/>
+      <c r="D147" s="36" t="s">
+        <v>143</v>
       </c>
       <c r="E147" s="27"/>
-      <c r="F147" s="30">
+      <c r="F147" s="29">
         <v>2.62</v>
       </c>
-      <c r="G147" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H147" s="30"/>
-      <c r="I147" s="30"/>
+      <c r="G147" s="29"/>
+      <c r="H147" s="29"/>
+      <c r="I147" s="29"/>
     </row>
     <row r="148" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="23"/>
       <c r="B148" s="23">
         <v>14.2</v>
       </c>
-      <c r="C148" s="30"/>
-      <c r="D148" s="38" t="s">
-        <v>150</v>
+      <c r="C148" s="29"/>
+      <c r="D148" s="36" t="s">
+        <v>144</v>
       </c>
       <c r="E148" s="27"/>
-      <c r="F148" s="30">
+      <c r="F148" s="29">
         <v>2.62</v>
       </c>
-      <c r="G148" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H148" s="30"/>
-      <c r="I148" s="30"/>
+      <c r="G148" s="29"/>
+      <c r="H148" s="29"/>
+      <c r="I148" s="29"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="23"/>
       <c r="B149" s="23">
         <v>14.3</v>
       </c>
-      <c r="C149" s="30"/>
-      <c r="D149" s="38" t="s">
-        <v>151</v>
+      <c r="C149" s="29"/>
+      <c r="D149" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="E149" s="27"/>
-      <c r="F149" s="30">
+      <c r="F149" s="29">
         <v>2.62</v>
       </c>
-      <c r="G149" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H149" s="30"/>
-      <c r="I149" s="30"/>
+      <c r="G149" s="29"/>
+      <c r="H149" s="29"/>
+      <c r="I149" s="29"/>
     </row>
     <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="23"/>
       <c r="B150" s="23">
         <v>14.4</v>
       </c>
-      <c r="C150" s="30"/>
-      <c r="D150" s="38" t="s">
-        <v>152</v>
+      <c r="C150" s="29"/>
+      <c r="D150" s="36" t="s">
+        <v>146</v>
       </c>
       <c r="E150" s="27"/>
-      <c r="F150" s="30">
+      <c r="F150" s="29">
         <v>2.62</v>
       </c>
-      <c r="G150" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H150" s="30"/>
-      <c r="I150" s="30"/>
+      <c r="G150" s="29"/>
+      <c r="H150" s="29"/>
+      <c r="I150" s="29"/>
     </row>
     <row r="151" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A151" s="23"/>
       <c r="B151" s="23">
         <v>14.5</v>
       </c>
-      <c r="C151" s="30"/>
-      <c r="D151" s="38" t="s">
-        <v>153</v>
+      <c r="C151" s="29"/>
+      <c r="D151" s="36" t="s">
+        <v>147</v>
       </c>
       <c r="E151" s="27"/>
-      <c r="F151" s="30">
+      <c r="F151" s="29">
         <v>2.62</v>
       </c>
-      <c r="G151" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H151" s="30"/>
-      <c r="I151" s="30"/>
+      <c r="G151" s="29"/>
+      <c r="H151" s="29"/>
+      <c r="I151" s="29"/>
     </row>
     <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="23"/>
       <c r="B152" s="23">
         <v>14.6</v>
       </c>
-      <c r="C152" s="30"/>
-      <c r="D152" s="38" t="s">
-        <v>154</v>
+      <c r="C152" s="29"/>
+      <c r="D152" s="36" t="s">
+        <v>148</v>
       </c>
       <c r="E152" s="27"/>
-      <c r="F152" s="30">
+      <c r="F152" s="29">
         <v>2.62</v>
       </c>
-      <c r="G152" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H152" s="30"/>
-      <c r="I152" s="30"/>
+      <c r="G152" s="29"/>
+      <c r="H152" s="29"/>
+      <c r="I152" s="29"/>
     </row>
     <row r="153" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="23"/>
       <c r="B153" s="23">
         <v>14.7</v>
       </c>
-      <c r="C153" s="30"/>
-      <c r="D153" s="38" t="s">
-        <v>155</v>
+      <c r="C153" s="29"/>
+      <c r="D153" s="36" t="s">
+        <v>149</v>
       </c>
       <c r="E153" s="27"/>
-      <c r="F153" s="30">
+      <c r="F153" s="29">
         <v>2.62</v>
       </c>
-      <c r="G153" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H153" s="30"/>
-      <c r="I153" s="30"/>
+      <c r="G153" s="29"/>
+      <c r="H153" s="29"/>
+      <c r="I153" s="29"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="23"/>
       <c r="B154" s="23">
         <v>14.8</v>
       </c>
-      <c r="C154" s="30"/>
-      <c r="D154" s="38" t="s">
-        <v>156</v>
+      <c r="C154" s="29"/>
+      <c r="D154" s="36" t="s">
+        <v>150</v>
       </c>
       <c r="E154" s="27"/>
-      <c r="F154" s="30">
+      <c r="F154" s="29">
         <v>2.62</v>
       </c>
-      <c r="G154" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H154" s="30"/>
-      <c r="I154" s="30"/>
+      <c r="G154" s="29"/>
+      <c r="H154" s="29"/>
+      <c r="I154" s="29"/>
     </row>
     <row r="155" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="23"/>
       <c r="B155" s="23">
         <v>14.9</v>
       </c>
-      <c r="C155" s="30"/>
-      <c r="D155" s="38" t="s">
-        <v>157</v>
+      <c r="C155" s="29"/>
+      <c r="D155" s="36" t="s">
+        <v>151</v>
       </c>
       <c r="E155" s="27"/>
-      <c r="F155" s="30">
+      <c r="F155" s="29">
         <v>2.62</v>
       </c>
-      <c r="G155" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H155" s="30"/>
-      <c r="I155" s="30"/>
+      <c r="G155" s="29"/>
+      <c r="H155" s="29"/>
+      <c r="I155" s="29"/>
     </row>
     <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="23"/>
-      <c r="B156" s="41">
+      <c r="B156" s="39">
         <v>14.1</v>
       </c>
-      <c r="C156" s="30"/>
-      <c r="D156" s="38" t="s">
-        <v>158</v>
+      <c r="C156" s="29"/>
+      <c r="D156" s="36" t="s">
+        <v>152</v>
       </c>
       <c r="E156" s="27"/>
-      <c r="F156" s="30">
+      <c r="F156" s="29">
         <v>2.62</v>
       </c>
-      <c r="G156" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H156" s="30"/>
-      <c r="I156" s="30"/>
+      <c r="G156" s="29"/>
+      <c r="H156" s="29"/>
+      <c r="I156" s="29"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A157" s="55"/>
-      <c r="B157" s="55"/>
-      <c r="C157" s="33"/>
-      <c r="D157" s="56"/>
-      <c r="E157" s="57"/>
-      <c r="F157" s="33"/>
-      <c r="G157" s="36"/>
-      <c r="H157" s="33"/>
-      <c r="I157" s="33"/>
+      <c r="A157" s="52"/>
+      <c r="B157" s="52"/>
+      <c r="C157" s="32"/>
+      <c r="D157" s="53"/>
+      <c r="E157" s="54"/>
+      <c r="F157" s="32"/>
+      <c r="G157" s="35"/>
+      <c r="H157" s="32"/>
+      <c r="I157" s="32"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A158" s="55"/>
-      <c r="B158" s="55"/>
-      <c r="C158" s="33"/>
-      <c r="D158" s="56"/>
-      <c r="E158" s="57"/>
-      <c r="F158" s="33"/>
-      <c r="G158" s="36"/>
-      <c r="H158" s="33"/>
-      <c r="I158" s="33"/>
+      <c r="A158" s="52"/>
+      <c r="B158" s="52"/>
+      <c r="C158" s="32"/>
+      <c r="D158" s="53"/>
+      <c r="E158" s="54"/>
+      <c r="F158" s="32"/>
+      <c r="G158" s="35"/>
+      <c r="H158" s="32"/>
+      <c r="I158" s="32"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="55"/>
-      <c r="B159" s="55"/>
-      <c r="C159" s="33"/>
-      <c r="D159" s="56"/>
-      <c r="E159" s="57"/>
-      <c r="F159" s="33"/>
-      <c r="G159" s="36"/>
-      <c r="H159" s="33"/>
-      <c r="I159" s="33"/>
+      <c r="A159" s="52"/>
+      <c r="B159" s="52"/>
+      <c r="C159" s="32"/>
+      <c r="D159" s="53"/>
+      <c r="E159" s="54"/>
+      <c r="F159" s="32"/>
+      <c r="G159" s="35"/>
+      <c r="H159" s="32"/>
+      <c r="I159" s="32"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G9:G13 G22:G47 G65:G70 G52:G61 G49:G50">
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16:G19">
-    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="52" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G78:G87">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G78)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G78)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G78)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="48" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G78)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G72:G76">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G72)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G72)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G72)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G90:G109">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G90)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G90)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G90)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G90)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G113:G116">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G113)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G113)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G113)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G113)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G119:G123">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G119)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G119)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G119)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G119)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G126:G131">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G126)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G126)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G126)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G126)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G134:G144">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G134)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G134)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G134)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G134)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",G48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F76">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",F76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",F76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",F76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",F76)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",F50)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",F50)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",F50)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",F50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F70">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FWL">
-      <formula>NOT(ISERROR(SEARCH("FWL",F70)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",F70)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",F70)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",F70)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>